<commit_message>
Assign and Unassigned succesful
</commit_message>
<xml_diff>
--- a/data/TEAM_AVAIL.xlsx
+++ b/data/TEAM_AVAIL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f5br38\github\LindeBasis\INM.App.CLI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDDE0CA5-E713-414A-A762-1B65E1C80742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F346068-CCEE-4806-93C1-8012173E4683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30315" yWindow="1515" windowWidth="21600" windowHeight="12645" xr2:uid="{AA243172-3DB3-445A-BB68-F471432CA2DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA243172-3DB3-445A-BB68-F471432CA2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="TEAM_AVAIL" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="162">
   <si>
     <t>ADID</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>sudipta.basak@linde.com</t>
-  </si>
-  <si>
-    <t>wfh</t>
   </si>
   <si>
     <t>IN08F9</t>
@@ -1354,9 +1351,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526001B4-6846-49F0-9FC7-503E16550939}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1407,7 +1417,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1427,173 +1437,173 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>44</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
         <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>53</v>
-      </c>
-      <c r="H11" t="s">
-        <v>54</v>
       </c>
       <c r="I11" t="s">
         <v>15</v>
@@ -1601,22 +1611,22 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>59</v>
-      </c>
-      <c r="G12" t="s">
-        <v>60</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -1627,28 +1637,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="G13" t="s">
-        <v>65</v>
-      </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
         <v>15</v>
@@ -1656,22 +1666,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>70</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
@@ -1682,25 +1692,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>76</v>
       </c>
-      <c r="G15" t="s">
-        <v>77</v>
-      </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -1708,129 +1718,129 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>80</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
         <v>81</v>
       </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>82</v>
-      </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
         <v>83</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>84</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>85</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>86</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>87</v>
       </c>
-      <c r="G17" t="s">
-        <v>88</v>
-      </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
         <v>89</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>90</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>92</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>93</v>
       </c>
-      <c r="G18" t="s">
-        <v>94</v>
-      </c>
       <c r="H18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>95</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>96</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>97</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>98</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>99</v>
       </c>
-      <c r="G19" t="s">
-        <v>100</v>
-      </c>
       <c r="H19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
         <v>101</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>102</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>103</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>105</v>
       </c>
-      <c r="G20" t="s">
-        <v>106</v>
-      </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" t="s">
         <v>15</v>
@@ -1838,77 +1848,77 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
         <v>107</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>109</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>110</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>111</v>
       </c>
-      <c r="G21" t="s">
-        <v>112</v>
-      </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>114</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>115</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>116</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>117</v>
       </c>
-      <c r="G22" t="s">
-        <v>118</v>
-      </c>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
         <v>119</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>120</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
         <v>121</v>
       </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>122</v>
       </c>
-      <c r="G23" t="s">
-        <v>123</v>
-      </c>
       <c r="H23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" t="s">
         <v>15</v>
@@ -1916,19 +1926,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
         <v>124</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>125</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>126</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>127</v>
-      </c>
-      <c r="G24" t="s">
-        <v>128</v>
       </c>
       <c r="H24" t="s">
         <v>14</v>
@@ -1939,19 +1949,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" t="s">
         <v>129</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>130</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>131</v>
       </c>
-      <c r="G25" t="s">
-        <v>132</v>
-      </c>
       <c r="H25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" t="s">
         <v>15</v>
@@ -1959,77 +1969,77 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
         <v>133</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>134</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>135</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>136</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>137</v>
       </c>
-      <c r="G26" t="s">
-        <v>138</v>
-      </c>
       <c r="H26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
         <v>139</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>140</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>141</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>142</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>143</v>
       </c>
-      <c r="G27" t="s">
-        <v>144</v>
-      </c>
       <c r="H27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
         <v>145</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>146</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>147</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>148</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>149</v>
       </c>
-      <c r="G28" t="s">
-        <v>150</v>
-      </c>
       <c r="H28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28" t="s">
         <v>15</v>
@@ -2037,25 +2047,25 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
         <v>151</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>152</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>153</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>154</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>155</v>
       </c>
-      <c r="G29" t="s">
-        <v>156</v>
-      </c>
       <c r="H29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I29" t="s">
         <v>15</v>
@@ -2063,28 +2073,28 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" t="s">
         <v>157</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>158</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>159</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>160</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>161</v>
       </c>
-      <c r="G30" t="s">
-        <v>162</v>
-      </c>
       <c r="H30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Team members list
Add full names Team members list
</commit_message>
<xml_diff>
--- a/data/TEAM_AVAIL.xlsx
+++ b/data/TEAM_AVAIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b2rt09\Downloads\INM.App.CLI-4.5\INM.App.CLI-4.5\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f5br38\github\LindeBasis\INM.App.CLI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BBBF6E-8227-4B92-9D59-31E019115B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F641F093-EAE2-4154-9FC6-C45453298D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AA243172-3DB3-445A-BB68-F471432CA2DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{AA243172-3DB3-445A-BB68-F471432CA2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="TEAM_AVAIL" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="180">
   <si>
     <t>ADID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>IN08C1</t>
   </si>
   <si>
-    <t>Imran</t>
-  </si>
-  <si>
     <t>Khan</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>IN11AA</t>
   </si>
   <si>
-    <t>Sudipta</t>
-  </si>
-  <si>
     <t>Basak</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>IN08F9</t>
   </si>
   <si>
-    <t>Santosh</t>
-  </si>
-  <si>
     <t>Kumar</t>
   </si>
   <si>
@@ -110,9 +101,6 @@
     <t>IN10F5</t>
   </si>
   <si>
-    <t>Abhijit</t>
-  </si>
-  <si>
     <t>Maiti</t>
   </si>
   <si>
@@ -122,9 +110,6 @@
     <t>IN1103</t>
   </si>
   <si>
-    <t>Sourav</t>
-  </si>
-  <si>
     <t>Biswas</t>
   </si>
   <si>
@@ -137,9 +122,6 @@
     <t>IN1130</t>
   </si>
   <si>
-    <t>Alok</t>
-  </si>
-  <si>
     <t>Tripathi</t>
   </si>
   <si>
@@ -149,9 +131,6 @@
     <t>F5BR38</t>
   </si>
   <si>
-    <t>Sumit</t>
-  </si>
-  <si>
     <t>Das</t>
   </si>
   <si>
@@ -161,9 +140,6 @@
     <t>IN1161</t>
   </si>
   <si>
-    <t>Deepjyoti</t>
-  </si>
-  <si>
     <t>Banerjee</t>
   </si>
   <si>
@@ -173,9 +149,6 @@
     <t>D1MT74</t>
   </si>
   <si>
-    <t>Rajiv</t>
-  </si>
-  <si>
     <t>rajiv.biswas@linde.com</t>
   </si>
   <si>
@@ -188,9 +161,6 @@
     <t>g3uw61</t>
   </si>
   <si>
-    <t>Raj</t>
-  </si>
-  <si>
     <t>raj.kumar@linde.com</t>
   </si>
   <si>
@@ -206,9 +176,6 @@
     <t>h1zj21</t>
   </si>
   <si>
-    <t xml:space="preserve">Utsha </t>
-  </si>
-  <si>
     <t>Rej</t>
   </si>
   <si>
@@ -221,9 +188,6 @@
     <t>h6pd38</t>
   </si>
   <si>
-    <t>Pankaj</t>
-  </si>
-  <si>
     <t>Singh</t>
   </si>
   <si>
@@ -239,12 +203,6 @@
     <t>g5dh34</t>
   </si>
   <si>
-    <t>SAMYUKTA</t>
-  </si>
-  <si>
-    <t>MAZUMDER</t>
-  </si>
-  <si>
     <t>samyukta.mazumder@linde.com</t>
   </si>
   <si>
@@ -257,9 +215,6 @@
     <t>g6ts81</t>
   </si>
   <si>
-    <t>Sajinur</t>
-  </si>
-  <si>
     <t>Khatun</t>
   </si>
   <si>
@@ -275,9 +230,6 @@
     <t xml:space="preserve">g3ne56 </t>
   </si>
   <si>
-    <t>Vivek</t>
-  </si>
-  <si>
     <t>vivek.kumar@linde.com</t>
   </si>
   <si>
@@ -290,9 +242,6 @@
     <t>h6gj64</t>
   </si>
   <si>
-    <t>Anirban</t>
-  </si>
-  <si>
     <t>Sardar</t>
   </si>
   <si>
@@ -308,9 +257,6 @@
     <t>g5gf56</t>
   </si>
   <si>
-    <t>Akash</t>
-  </si>
-  <si>
     <t>Bhattacharjee</t>
   </si>
   <si>
@@ -326,9 +272,6 @@
     <t>g0mz79</t>
   </si>
   <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
     <t>Kaintura</t>
   </si>
   <si>
@@ -344,9 +287,6 @@
     <t>g5kt53</t>
   </si>
   <si>
-    <t>Shaik</t>
-  </si>
-  <si>
     <t>Alenoor</t>
   </si>
   <si>
@@ -362,9 +302,6 @@
     <t>g3uh23</t>
   </si>
   <si>
-    <t>Preity</t>
-  </si>
-  <si>
     <t>Mishra</t>
   </si>
   <si>
@@ -380,9 +317,6 @@
     <t>g8hq15</t>
   </si>
   <si>
-    <t>Arpan</t>
-  </si>
-  <si>
     <t>Halder</t>
   </si>
   <si>
@@ -410,9 +344,6 @@
     <t>H6UC13</t>
   </si>
   <si>
-    <t>Sreejita</t>
-  </si>
-  <si>
     <t>Bose</t>
   </si>
   <si>
@@ -422,9 +353,6 @@
     <t>e2ca12</t>
   </si>
   <si>
-    <t>Nabojita</t>
-  </si>
-  <si>
     <t>Ghosh</t>
   </si>
   <si>
@@ -440,9 +368,6 @@
     <t>g3ju81</t>
   </si>
   <si>
-    <t>Shreyashee</t>
-  </si>
-  <si>
     <t>Majumder</t>
   </si>
   <si>
@@ -458,9 +383,6 @@
     <t>h2jw05</t>
   </si>
   <si>
-    <t xml:space="preserve">Adarsh </t>
-  </si>
-  <si>
     <t>Rana</t>
   </si>
   <si>
@@ -476,9 +398,6 @@
     <t>h6va73</t>
   </si>
   <si>
-    <t>Dwaipayan</t>
-  </si>
-  <si>
     <t>Bhattacharyya</t>
   </si>
   <si>
@@ -494,9 +413,6 @@
     <t>G5YD42</t>
   </si>
   <si>
-    <t>Sudip</t>
-  </si>
-  <si>
     <t>Chowdhury</t>
   </si>
   <si>
@@ -512,30 +428,15 @@
     <t>g7vq68</t>
   </si>
   <si>
-    <t>Rajarshi</t>
-  </si>
-  <si>
     <t>Rakshit</t>
   </si>
   <si>
     <t>f1cs12@linde.com</t>
   </si>
   <si>
-    <t>Ivan</t>
-  </si>
-  <si>
     <t>SK</t>
   </si>
   <si>
-    <t>Andrej</t>
-  </si>
-  <si>
-    <t>Pavol</t>
-  </si>
-  <si>
-    <t>Michal</t>
-  </si>
-  <si>
     <t>Gaal</t>
   </si>
   <si>
@@ -570,6 +471,108 @@
   </si>
   <si>
     <t>d7nd84@linde.com</t>
+  </si>
+  <si>
+    <t>Mazumder</t>
+  </si>
+  <si>
+    <t>Imran Khan Patan</t>
+  </si>
+  <si>
+    <t>Sudipta  Basak</t>
+  </si>
+  <si>
+    <t>Santosh  Kumar</t>
+  </si>
+  <si>
+    <t>Abhijit  Maiti</t>
+  </si>
+  <si>
+    <t>Sourav  Biswas</t>
+  </si>
+  <si>
+    <t>Alok Kumar Tripathi</t>
+  </si>
+  <si>
+    <t>Sumit  Das</t>
+  </si>
+  <si>
+    <t>Deepjyoti  Banerjee</t>
+  </si>
+  <si>
+    <t>Rajiv  Biswas</t>
+  </si>
+  <si>
+    <t>Raj  Kumar</t>
+  </si>
+  <si>
+    <t>Utsha   Rej</t>
+  </si>
+  <si>
+    <t>Pankaj Kumar Singh</t>
+  </si>
+  <si>
+    <t>Samyukta  Mazumder</t>
+  </si>
+  <si>
+    <t>Sajinur  Khatun</t>
+  </si>
+  <si>
+    <t>Vivek  Kumar</t>
+  </si>
+  <si>
+    <t>Anirban  Sardar</t>
+  </si>
+  <si>
+    <t>Akash  Bhattacharjee</t>
+  </si>
+  <si>
+    <t>Abhishek  Kaintura</t>
+  </si>
+  <si>
+    <t>Shaik  Alenoor</t>
+  </si>
+  <si>
+    <t>Preity  Mishra</t>
+  </si>
+  <si>
+    <t>Arpan  Halder</t>
+  </si>
+  <si>
+    <t>Sourav  Roy</t>
+  </si>
+  <si>
+    <t>Sreejita  Bose</t>
+  </si>
+  <si>
+    <t>Nabojita  Ghosh</t>
+  </si>
+  <si>
+    <t>Shreyashee  Majumder</t>
+  </si>
+  <si>
+    <t>Adarsh   Rana</t>
+  </si>
+  <si>
+    <t>Dwaipayan  Bhattacharyya</t>
+  </si>
+  <si>
+    <t>Sudip  Chowdhury</t>
+  </si>
+  <si>
+    <t>Rajarshi  Rakshit</t>
+  </si>
+  <si>
+    <t>Ivan  Gaal</t>
+  </si>
+  <si>
+    <t>Andrej  Meszaros</t>
+  </si>
+  <si>
+    <t>Pavol  Jezko</t>
+  </si>
+  <si>
+    <t>Michal  Balaz</t>
   </si>
 </sst>
 </file>
@@ -1036,9 +1039,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1416,24 +1418,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526001B4-6846-49F0-9FC7-503E16550939}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N32" activeCellId="1" sqref="I27 N32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1462,784 +1465,784 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" t="s">
+        <v>117</v>
+      </c>
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" t="s">
         <v>14</v>
       </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" t="s">
         <v>14</v>
       </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I31" t="s">
         <v>14</v>
       </c>
-      <c r="I8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" t="s">
+        <v>143</v>
+      </c>
+      <c r="H32" t="s">
+        <v>133</v>
+      </c>
+      <c r="I32" t="s">
         <v>14</v>
       </c>
-      <c r="I9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" t="s">
+        <v>144</v>
+      </c>
+      <c r="H33" t="s">
+        <v>133</v>
+      </c>
+      <c r="I33" t="s">
         <v>14</v>
       </c>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I34" t="s">
         <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" t="s">
-        <v>76</v>
-      </c>
-      <c r="H15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" t="s">
-        <v>121</v>
-      </c>
-      <c r="G23" t="s">
-        <v>122</v>
-      </c>
-      <c r="H23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H25" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" t="s">
-        <v>136</v>
-      </c>
-      <c r="G26" t="s">
-        <v>137</v>
-      </c>
-      <c r="H26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D27" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" t="s">
-        <v>142</v>
-      </c>
-      <c r="G27" t="s">
-        <v>143</v>
-      </c>
-      <c r="H27" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" t="s">
-        <v>149</v>
-      </c>
-      <c r="H28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" t="s">
-        <v>155</v>
-      </c>
-      <c r="H29" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" t="s">
-        <v>158</v>
-      </c>
-      <c r="D30" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" t="s">
-        <v>160</v>
-      </c>
-      <c r="G30" t="s">
-        <v>161</v>
-      </c>
-      <c r="H30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" t="s">
-        <v>162</v>
-      </c>
-      <c r="F31" t="s">
-        <v>167</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H31" t="s">
-        <v>163</v>
-      </c>
-      <c r="I31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>172</v>
-      </c>
-      <c r="D32" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>173</v>
-      </c>
-      <c r="D33" t="s">
-        <v>165</v>
-      </c>
-      <c r="F33" t="s">
-        <v>175</v>
-      </c>
-      <c r="G33" t="s">
-        <v>177</v>
-      </c>
-      <c r="H33" t="s">
-        <v>163</v>
-      </c>
-      <c r="I33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>174</v>
-      </c>
-      <c r="D34" t="s">
-        <v>166</v>
-      </c>
-      <c r="F34" t="s">
-        <v>169</v>
-      </c>
-      <c r="G34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H34" t="s">
-        <v>163</v>
-      </c>
-      <c r="I34" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2248,6 +2251,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="921b7353-8eee-4d57-95e7-6707d4aafa1b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100425AA63552E6DD44A4776F0079EC1931" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bb2ddc56d56984fce5cbace59b9ded1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee" xmlns:ns3="90beab9b-5c97-49ef-80e1-8bede52b6c41" xmlns:ns4="921b7353-8eee-4d57-95e7-6707d4aafa1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06b5fce8f723d0c680f9511fcc7dd520" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee"/>
@@ -2507,34 +2530,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="921b7353-8eee-4d57-95e7-6707d4aafa1b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88DF22D8-BD38-4BDA-A92B-220A271182FD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A67DE999-3626-4271-B2F3-B465CB9CDD4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee"/>
+    <ds:schemaRef ds:uri="921b7353-8eee-4d57-95e7-6707d4aafa1b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76CAEA75-AC20-4C41-BD0C-0114A0E16144}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76CAEA75-AC20-4C41-BD0C-0114A0E16144}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A67DE999-3626-4271-B2F3-B465CB9CDD4C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88DF22D8-BD38-4BDA-A92B-220A271182FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5a40e1f1-7edf-47f8-ade6-3fa40173a7ee"/>
+    <ds:schemaRef ds:uri="90beab9b-5c97-49ef-80e1-8bede52b6c41"/>
+    <ds:schemaRef ds:uri="921b7353-8eee-4d57-95e7-6707d4aafa1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>